<commit_message>
using xlsx to log the excel sheet as json
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhack\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49E1589A-5DB3-477F-B3D9-D7D95639C78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA02D4BB-284C-4508-886D-4AB4D5F78EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{28CA0B5F-4C06-435A-968E-C3051D3CC4FE}"/>
+    <workbookView xWindow="3810" yWindow="1290" windowWidth="21600" windowHeight="11385" xr2:uid="{97C91E3A-7054-4F87-A57B-4DD5A64BB17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,62 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Midmarket</t>
+  </si>
+  <si>
+    <t>Channel Partners</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Carretera</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Discount Band</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Units Sold</t>
+  </si>
+  <si>
+    <t>Manufacturing P</t>
+  </si>
+  <si>
+    <t>US$  3.00</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,13 +436,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2463D616-4347-4728-A165-689B328DE437}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545F25EC-9D4A-44F8-BFFB-3012101AA3D6}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>1618.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1321</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>2178</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>888</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>2470</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>1513</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>921</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>2518</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>